<commit_message>
reparando reporte de compras
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/compras.xlsx
+++ b/public/application/files/jasper/templates/compras.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14200" tabRatio="198"/>
+    <workbookView xWindow="-24240" yWindow="0" windowWidth="25120" windowHeight="14200" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>{compania:nombre}</t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>Compras</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>IEPS</t>
+  </si>
+  <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -297,8 +309,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -340,19 +356,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -366,8 +370,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -381,6 +397,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -394,6 +412,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -841,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K3"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -853,165 +873,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="29.75" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" ht="29.75" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="29.75" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="14"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" ht="22.25" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" ht="22.25" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="22.25" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="22.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7" t="s">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="22.25" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" ht="18">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
@@ -1032,10 +1052,10 @@
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
@@ -1061,46 +1081,55 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="K12" s="4" t="s">
+    <row r="14" spans="1:11">
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="K13" s="4" t="s">
+    <row r="15" spans="1:11">
+      <c r="J15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="K14" s="4" t="s">
+    <row r="16" spans="1:11">
+      <c r="J16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="K15" s="4" t="s">
+    <row r="17" spans="10:11">
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="25">
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A9:I9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A9:I9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
@@ -1108,9 +1137,13 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>